<commit_message>
table: attributes_system change Sel3 to have 36 points
</commit_message>
<xml_diff>
--- a/FC_tables/Attributes/Attributes_system.xlsx
+++ b/FC_tables/Attributes/Attributes_system.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24827"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAC49001-06D5-4B85-92AE-ADBDF22C8C67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="20370" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -17,8 +18,8 @@
 </file>
 
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
-<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <connection id="1" name="dsfsdfs" type="6" refreshedVersion="5" background="1" saveData="1">
+<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16">
+  <connection id="1" xr16:uid="{00000000-0015-0000-FFFF-FFFF00000000}" name="dsfsdfs" type="6" refreshedVersion="5" background="1" saveData="1">
     <textPr codePage="437" sourceFile="C:\Users\Silver Wolf\Desktop\dsfsdfs.txt" delimited="0">
       <textFields count="6">
         <textField/>
@@ -99,7 +100,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -149,7 +150,7 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="dsfsdfs" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="dsfsdfs" connectionId="1" xr16:uid="{00000000-0016-0000-0000-000000000000}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -228,6 +229,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -263,6 +281,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -438,11 +473,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M13" sqref="M13"/>
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -537,10 +572,10 @@
         <v>13</v>
       </c>
       <c r="F4">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="G4">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>